<commit_message>
BIS-772: Working on XLS export. Added one more PropertyTypePermId to the list of selected fields to improve sorting check.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/systemtest/asapi/v3/test_files/xls/export/export-sample-filtered-fields.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/systemtest/asapi/v3/test_files/xls/export/export-sample-filtered-fields.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">SAMPLE</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organism</t>
   </si>
   <si>
     <t xml:space="preserve">FV-TEST</t>
@@ -106,6 +109,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -178,16 +182,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -208,100 +216,103 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
+      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16379" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16379" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="M4" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="H5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="J5" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>